<commit_message>
Report is done. Added comments.
</commit_message>
<xml_diff>
--- a/Epam_Task7/Resources/Report1.xlsx
+++ b/Epam_Task7/Resources/Report1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\learn\C#\EPAM\EPAM_Task7\Task7\Epam_Task7\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0E3DD4E8-888F-43CB-80B9-566768B17880}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{FE0BB052-2EA2-4E87-BF11-86D2CF9F8716}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="8304" xr2:uid="{6423FB5D-CAE2-43E5-99B2-925565F7D6D2}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="8304" xr2:uid="{98B942C3-A48A-4C7D-9914-5CB8E831F08C}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Session</t>
   </si>
@@ -38,12 +38,6 @@
   <si>
     <t>_x000D_
 Engineer system programmer</t>
-  </si>
-  <si>
-    <t>Software engineer</t>
-  </si>
-  <si>
-    <t>electronics engineer</t>
   </si>
 </sst>
 </file>
@@ -398,8 +392,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F667100-049A-415F-8A6F-1E71E07A4EC3}">
-  <dimension ref="A1:C4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C55D410-5FC7-4B68-829B-01B325A47C4F}">
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -427,28 +421,6 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4">
-        <v>5.75</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>